<commit_message>
added problems text file
</commit_message>
<xml_diff>
--- a/Data/Exercises Features.xlsx
+++ b/Data/Exercises Features.xlsx
@@ -453,7 +453,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[[[37, 27, 18, 162, 171, 174, 156, 118, 114, 24, 26, 127, 143]], [[34, 54, 45, 160, 166, 175, 162, 157, 157, 36, 40, 126, 138]], [[34, 40, 31, 160, 166, 179, 167, 132, 131, 30, 33, 137, 148]]]</t>
+          <t>[[31, 34, 8, 158, 175, 159, 129, 97, 113, 15, 27, 95, 153], [34, 47, 29, 167, 179, 178, 162, 142, 148, 23, 35, 114, 133], [33, 32, 24, 163, 162, 179, 178, 122, 121, 20, 26, 122, 137]]</t>
         </is>
       </c>
     </row>
@@ -465,7 +465,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>[[[42, 123, 121, 116, 61, 120, 149, 158, 161, 158, 156, 123, 107]], [[46, 113, 120, 116, 68, 118, 133, 164, 158, 154, 60, 115, 162]], [[45, 111, 116, 85, 57, 139, 138, 164, 167, 150, 138, 115, 108]]]</t>
+          <t>[[45, 110, 120, 68, 48, 28, 148, 171, 174, 171, 169, 123, 119], [42, 107, 116, 76, 53, 61, 141, 174, 163, 167, 61, 124, 140], [45, 109, 115, 84, 62, 145, 133, 174, 172, 158, 145, 117, 100]]</t>
         </is>
       </c>
     </row>
@@ -477,7 +477,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>[[[38, 178, 28, 179, 17, 168, 169, 156, 100, 158, 55, 127, 178]], [[7, 162, 37, 166, 67, 177, 145, 117, 109, 58, 56, 107, 176]], [[2, 154, 23, 156, 102, 159, 146, 146, 143, 109, 115, 93, 151]]]</t>
+          <t>[[25, 176, 37, 165, 58, 165, 113, 155, 127, 125, 110, 82, 92], [21, 172, 48, 137, 102, 68, 140, 133, 92, 98, 46, 164, 130], [12, 158, 63, 170, 30, 134, 168, 127, 94, 98, 43, 79, 138]]</t>
         </is>
       </c>
     </row>

</xml_diff>